<commit_message>
Update automatico via Actualizar 04-30-2020 18-55-02
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
+++ b/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22823"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00D0E3A7-7983-4476-9668-D009A4236A34}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm.Criteria" localSheetId="0">[1]Hoja1!$AC$2:$AC$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Fuente</t>
   </si>
@@ -74,52 +74,55 @@
     <t>División administrativa</t>
   </si>
   <si>
+    <t>Poder Judicial de Honduras</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>La potestad de impartir justicia emana del pueblo y se imparte gratuitamente en nombre del Estado, por magistrados y jueces independientes, únicamente sometidos a la Constitución y a las leyes. El Poder Judicial se integra por una Corte Suprema de Justicia, por las Cortes de Apelaciones, los Juzgados, y demás dependencias que señale la Ley</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=comunicado-del-poder-judicial</t>
+  </si>
+  <si>
+    <t>Se autoriza para que todo Servidor Judicial mayor a 60 años de edad, permanezca en su
+casa y que, dependiendo de la naturaleza de las tareas asignadas, el trabajo bajo su
+responsabilidad pueda desarrollarlo de manera remota a través de las plataformas
+informáticas disponibles o de la forma como sea indicada por su superior jerárquico.</t>
+  </si>
+  <si>
+    <t>15/3/2020</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
     <t>Dirección del trabajo</t>
   </si>
   <si>
-    <t>Trabajo</t>
-  </si>
-  <si>
     <t>La Dirección del Trabajo es un Servicio Público descentralizado, con personalidad jurídica y patrimonio propio. Está sometido a la supervigilancia del Presidente de la República a través del Ministerio del Trabajo y Previsión Social, y se rige por su Ley Orgánica (D.F.L. Nº 2, del 30 de mayo de 1967) y el D.L. Nº 3.501 de 1981.</t>
   </si>
   <si>
-    <t>https://www.dt.gob.cl/legislacion/1624/articles-118468_recurso_pdf.pdf</t>
-  </si>
-  <si>
-    <t>complementa doctrina contenida en dictámenes N°1116/004 y N°1239/005 que fijan criterios y orientaciones sobre el impacto, en materia laboral, de la emergencia sanitaria provocada por el virus Covid-19.</t>
+    <t>https://www.dt.gob.cl/legislacion/1624/articles-118469_recurso_pdf.pdf</t>
   </si>
   <si>
     <t>https://www.dt.gob.cl/legislacion/1624/w3-channel.html</t>
   </si>
   <si>
-    <t>22/03/202</t>
-  </si>
-  <si>
     <t>Chile</t>
   </si>
   <si>
     <t>Ministerial</t>
   </si>
   <si>
-    <t>https://www.dt.gob.cl/legislacion/1624/articles-118469_recurso_pdf.pdf</t>
-  </si>
-  <si>
-    <t>Complementa doctrina contenida en Dictamen N°1116/004, de 06.03.2020, que fija criterios y orientaciones sobre el impacto, en materia laboral, de la emergencia sanitaria provocada por el virus Covid-19, en el sentido que indica.</t>
-  </si>
-  <si>
     <t>Instituto de seguridad laboral</t>
   </si>
   <si>
     <t>El Instituto de Seguridad Laboral, es la entidad pública encargada de administrar el Seguro Social contra Riesgos de Accidentes del Trabajo y Enfermedades Profesionales. Es un servicio público que pertenece al Ministerio del Trabajo y Previsión Social, y a través de su actuar genera Valor Público otorgando Calidad de Vida a los y las trabajadores/as</t>
   </si>
   <si>
-    <t>Contacto de consultas y envío de antecedentes</t>
-  </si>
-  <si>
     <t>https://www.isl.gob.cl/covid-19/</t>
-  </si>
-  <si>
-    <t>Información para usuarios referente al COVID-19.</t>
   </si>
   <si>
     <t>Instituto de previsión social</t>
@@ -144,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,7 +271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -312,14 +315,19 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -339,6 +347,99 @@
         <bottom style="thin">
           <color theme="4"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
       </border>
     </dxf>
     <dxf>
@@ -392,32 +493,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -461,32 +536,6 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -541,70 +590,68 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -639,44 +686,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -742,29 +751,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
   <autoFilter ref="A1:K7" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <tableColumns count="11">
-    <tableColumn id="2" xr3:uid="{A60CF310-D129-4744-AE47-EA0A16C6004B}" name="Fuente" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{CC100997-5BD5-48A6-8DA1-3E422557046E}" name="ID_Dato " dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{A60CF310-D129-4744-AE47-EA0A16C6004B}" name="Fuente" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{CC100997-5BD5-48A6-8DA1-3E422557046E}" name="ID_Dato " dataDxfId="9">
       <calculatedColumnFormula>+ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{20395840-3BEC-4C3C-AA9D-B15B82B91B23}" name="Categoria" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{3882ED5F-9896-4D6A-94FA-91141D829E29}" name="Descripción Fuente" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{5B662778-AFCE-45AF-BA5E-8EE75434DCE2}" name="Descarga Link" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{F19A1719-601F-4207-A7A5-1C7177A726DF}" name="Descripción información" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{C428BE36-6D12-4F4C-937B-4D9B2BE733CB}" name="Sitio Web" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{8A64974B-7039-4EC2-86FD-F906B25B65C5}" name="Fecha consulta" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{76A5A7F7-E8CD-4AD7-BD38-521CEC7FA43D}" name="Fecha publicación" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{C1BACFD5-672A-458F-A24A-AF2164F6B966}" name="País" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{CBA3644C-97A1-4B18-A3FF-89F9754FAC27}" name="División administrativa" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{20395840-3BEC-4C3C-AA9D-B15B82B91B23}" name="Categoria" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{3882ED5F-9896-4D6A-94FA-91141D829E29}" name="Descripción Fuente" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{5B662778-AFCE-45AF-BA5E-8EE75434DCE2}" name="Descarga Link" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{F19A1719-601F-4207-A7A5-1C7177A726DF}" name="Descripción información" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{C428BE36-6D12-4F4C-937B-4D9B2BE733CB}" name="Sitio Web" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{8A64974B-7039-4EC2-86FD-F906B25B65C5}" name="Fecha consulta" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{76A5A7F7-E8CD-4AD7-BD38-521CEC7FA43D}" name="Fecha publicación" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{C1BACFD5-672A-458F-A24A-AF2164F6B966}" name="País" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{CBA3644C-97A1-4B18-A3FF-89F9754FAC27}" name="División administrativa" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1062,23 +1071,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="69.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.21875" customWidth="1"/>
-    <col min="6" max="6" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="55.28515625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="22.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="31.9" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="61.9" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
@@ -1127,32 +1138,28 @@
       <c r="D2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="10">
-        <v>43917</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="K2" s="4"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="61.9" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6">
         <f t="shared" ref="B3:B7" si="0">+ROW()-1</f>
@@ -1162,16 +1169,14 @@
         <v>12</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="H3" s="10">
         <v>43917</v>
@@ -1180,16 +1185,16 @@
         <v>43909</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="61.9" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="6">
         <f t="shared" si="0"/>
@@ -1199,29 +1204,27 @@
         <v>12</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="14" t="s">
-        <v>24</v>
-      </c>
+      <c r="F4" s="14"/>
       <c r="G4" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="11">
         <v>43917</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="61.9" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" s="6">
         <f t="shared" si="0"/>
@@ -1231,27 +1234,25 @@
         <v>12</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="11">
         <v>43917</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="61.9" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>27</v>
       </c>
@@ -1277,15 +1278,15 @@
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="57.6">
+      <c r="A7" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>11</v>
       </c>
       <c r="B7" s="6">
         <f t="shared" si="0"/>
@@ -1295,7 +1296,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="14" t="s">
@@ -1309,10 +1310,10 @@
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1324,13 +1325,14 @@
     <hyperlink ref="G5" r:id="rId2" xr:uid="{0FD97349-53B2-48F9-8FB0-F36688365579}"/>
     <hyperlink ref="G6" r:id="rId3" display="https://www.ips.gob.cl/servlet/internet/noticia/1421810692952/locales-pago-operativos-sabado28-domingo29-marzo" xr:uid="{153699C3-67F5-46C6-BDEF-5E8F5CECE9F1}"/>
     <hyperlink ref="G3" r:id="rId4" xr:uid="{D1B9B175-F438-42C7-8F26-AE7262E7E1F0}"/>
-    <hyperlink ref="G2" r:id="rId5" xr:uid="{B1928BF5-9CB8-4591-A4FC-29C12CC65520}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{2D719A1D-601A-43CF-BFD7-DA6E329D9F90}"/>
-    <hyperlink ref="G7" r:id="rId7" xr:uid="{A81D850A-A085-4232-A1D2-7280F93E1078}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{2D719A1D-601A-43CF-BFD7-DA6E329D9F90}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{A81D850A-A085-4232-A1D2-7280F93E1078}"/>
+    <hyperlink ref="G2" r:id="rId7" xr:uid="{89832B8C-46B1-4E3A-B226-0588FB37741C}"/>
+    <hyperlink ref="E2" r:id="rId8" xr:uid="{44E5BE55-9BE8-4C19-8EB2-4729F3ABC777}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 04-30-2020 20-18-53
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
+++ b/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00D0E3A7-7983-4476-9668-D009A4236A34}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3914FBDB-80B1-4D6F-B64F-6F69A49DACD2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Fuente</t>
   </si>
@@ -98,43 +98,81 @@
     <t>Honduras</t>
   </si>
   <si>
+    <t>Ministerial</t>
+  </si>
+  <si>
+    <t>SINAGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El Sistema Nacional de Gestión de Riesgos (SINAGER) se
+regulará en un marco institucional, el cual comprenderá a todos los sectores de la sociedad hondureña, tales sectores son el público y el privado. LEY DEL SISTEMA NACIONAL DE GESTIÓN DE RIESGOS (SINAGER)  se definirán, planificarán y ejecutarán todas las acciones relacionadas con la prevención, adaptación al cambio climático y a otro tipo de eventos, manejo financiero del riesgo de desastres, preparación permanente y efectiva, la asistencia de ayuda humanitaria en caso de desastres y emergencia, a la rehabilitación y reconstrucción de las zonas afectadas por desastres.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=Se-suspenden-labores-en-el-sector-Publico-y-Privado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Se suspenden labores en el sector Público y Privado.
+2) Se prohíben eventos de todo tipo y número de personas.
+3) Se cancela toda actividades deportivas, cultural y sociales.
+4) Se prohíbe el funcionamiento del Transporte público.
+5) Se suspenden las celebraciones religiosas presenciales.
+6) Se cierran todos los negocios incluyendo centros comerciales.
+7) Se cierran las fronteras aéreas, terrestres y marítimas en todo el territorio nacional. </t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=Comunicados&amp;page=10</t>
+  </si>
+  <si>
+    <t>Ministerio Público</t>
+  </si>
+  <si>
+    <t>El Ministerio Público (Fiscalía General o Procuraduría) es un organismo Público generalmente estatal, al que se atribuye, dentro de un estado de Derecho democrático la representación de los intereses de la sociedad mediante el ejercicio de las facultades de dirección de la investigación.</t>
+  </si>
+  <si>
+    <t>El Ministerio Público, ante la Alerta Roja para todo el país como medida para evitar el COVID-19 (Coronavirus), INFORMA LO SIGUIENTE:
+ Suspender las labores a nivel nacional para todo el personal que labora en las diferentes oficinas desde este lunes 16 de marzo a las 12:00 horas hasta el próximo domingo 22 de marzo a las 23:59:59 horas; Se exceptúa de esa disposición a todo aquel empleado que tengan que desarrollar actividades previas o planificadas con anticipación, tales como: turnos y otras inherentes al normal desempeño de esta Institución.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=comunicado-del-ministerio-publico</t>
+  </si>
+  <si>
+    <t>16/3/2020</t>
+  </si>
+  <si>
+    <t>Instituto de seguridad laboral</t>
+  </si>
+  <si>
+    <t>El Instituto de Seguridad Laboral, es la entidad pública encargada de administrar el Seguro Social contra Riesgos de Accidentes del Trabajo y Enfermedades Profesionales. Es un servicio público que pertenece al Ministerio del Trabajo y Previsión Social, y a través de su actuar genera Valor Público otorgando Calidad de Vida a los y las trabajadores/as</t>
+  </si>
+  <si>
+    <t>https://www.isl.gob.cl/covid-19/</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>secretaría de Gobernación Justicia y Desentralización</t>
+  </si>
+  <si>
+    <t>Ante la emergencia nacional como prevención ante el COVID-19, se realizó
+la suspensión de labores en dichas Dependencias a partir del lunes dieciséis
+(16) al viernes veinte (20) de marzo del presente año.
+Los días antes mencionados se declaran INHÁBILES para los efectos, plazos,
+actuaciones y términos legales que la Ley establece, los cuales quedan
+suspendidos empezando a correr nuevamente los términos legales a partir
+del primer día hábil.</t>
+  </si>
+  <si>
+    <t>Locales de pago pensionados, sucursales abiertas (Sábado 28 y Domingo 29 Marzo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ips.gob.cl/servlet/internet/noticia/1421810692952/locales-pago-operativos-sabado28-domingo29-marzo </t>
+  </si>
+  <si>
     <t>Dirección del trabajo</t>
   </si>
   <si>
     <t>La Dirección del Trabajo es un Servicio Público descentralizado, con personalidad jurídica y patrimonio propio. Está sometido a la supervigilancia del Presidente de la República a través del Ministerio del Trabajo y Previsión Social, y se rige por su Ley Orgánica (D.F.L. Nº 2, del 30 de mayo de 1967) y el D.L. Nº 3.501 de 1981.</t>
-  </si>
-  <si>
-    <t>https://www.dt.gob.cl/legislacion/1624/articles-118469_recurso_pdf.pdf</t>
-  </si>
-  <si>
-    <t>https://www.dt.gob.cl/legislacion/1624/w3-channel.html</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>Ministerial</t>
-  </si>
-  <si>
-    <t>Instituto de seguridad laboral</t>
-  </si>
-  <si>
-    <t>El Instituto de Seguridad Laboral, es la entidad pública encargada de administrar el Seguro Social contra Riesgos de Accidentes del Trabajo y Enfermedades Profesionales. Es un servicio público que pertenece al Ministerio del Trabajo y Previsión Social, y a través de su actuar genera Valor Público otorgando Calidad de Vida a los y las trabajadores/as</t>
-  </si>
-  <si>
-    <t>https://www.isl.gob.cl/covid-19/</t>
-  </si>
-  <si>
-    <t>Instituto de previsión social</t>
-  </si>
-  <si>
-    <t>El Instituto de Previsión Social (IPS), es un servicio público creado a partir del artículo 53 de la Ley 20.255, de Reforma al Sistema Previsional, descentralizado, y con personalidad jurídica y patrimonio propio. El IPS desarrolla sus funciones bajo la supervigilancia del Presidente de la República, a través del Ministerio del Trabajo, por intermedio de la Subsecretaría de Previsión Social. Este servicio tiene por objetivo la administración del sistema de pensiones solidarias y de los regímenes previsionales administrados anteriormente por el ex INP, y constituye un servicio público regido por el Sistema de Alta Dirección Pública, establecido en la ley N° 19.882.</t>
-  </si>
-  <si>
-    <t>Locales de pago pensionados, sucursales abiertas (Sábado 28 y Domingo 29 Marzo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.ips.gob.cl/servlet/internet/noticia/1421810692952/locales-pago-operativos-sabado28-domingo29-marzo </t>
   </si>
   <si>
     <t>Centro de consultas COVID-19, preguntas frecuentes.</t>
@@ -271,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -290,9 +328,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1071,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1125,7 +1160,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="6">
@@ -1135,31 +1170,33 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A3" s="12" t="s">
-        <v>18</v>
+      <c r="A3" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="6">
         <f t="shared" ref="B3:B7" si="0">+ROW()-1</f>
@@ -1168,32 +1205,32 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="9" t="s">
+      <c r="E3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="10">
-        <v>43917</v>
-      </c>
-      <c r="I3" s="10">
-        <v>43909</v>
+      <c r="F3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="6">
@@ -1203,28 +1240,32 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="9" t="s">
+      <c r="E4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="11">
-        <v>43917</v>
-      </c>
-      <c r="I4" s="5"/>
+      <c r="G4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="J4" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A5" s="12" t="s">
-        <v>24</v>
+      <c r="A5" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="B5" s="6">
         <f t="shared" si="0"/>
@@ -1233,28 +1274,28 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="11">
+      <c r="D5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="10">
         <v>43917</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A6" s="12" t="s">
-        <v>27</v>
+      <c r="A6" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B6" s="6">
         <f t="shared" si="0"/>
@@ -1263,30 +1304,30 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="11">
+      <c r="D6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="10">
         <v>43917</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57.6">
-      <c r="A7" s="12" t="s">
-        <v>18</v>
+      <c r="A7" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B7" s="6">
         <f t="shared" si="0"/>
@@ -1295,25 +1336,25 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="11">
+      <c r="D7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="10">
         <v>43917</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1321,18 +1362,19 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C7" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{37B1EE56-288C-41B0-9515-9EE240BD31D5}"/>
-    <hyperlink ref="G5" r:id="rId2" xr:uid="{0FD97349-53B2-48F9-8FB0-F36688365579}"/>
-    <hyperlink ref="G6" r:id="rId3" display="https://www.ips.gob.cl/servlet/internet/noticia/1421810692952/locales-pago-operativos-sabado28-domingo29-marzo" xr:uid="{153699C3-67F5-46C6-BDEF-5E8F5CECE9F1}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{D1B9B175-F438-42C7-8F26-AE7262E7E1F0}"/>
-    <hyperlink ref="G4" r:id="rId5" xr:uid="{2D719A1D-601A-43CF-BFD7-DA6E329D9F90}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{A81D850A-A085-4232-A1D2-7280F93E1078}"/>
-    <hyperlink ref="G2" r:id="rId7" xr:uid="{89832B8C-46B1-4E3A-B226-0588FB37741C}"/>
-    <hyperlink ref="E2" r:id="rId8" xr:uid="{44E5BE55-9BE8-4C19-8EB2-4729F3ABC777}"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{0FD97349-53B2-48F9-8FB0-F36688365579}"/>
+    <hyperlink ref="G6" r:id="rId2" display="https://www.ips.gob.cl/servlet/internet/noticia/1421810692952/locales-pago-operativos-sabado28-domingo29-marzo" xr:uid="{153699C3-67F5-46C6-BDEF-5E8F5CECE9F1}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{A81D850A-A085-4232-A1D2-7280F93E1078}"/>
+    <hyperlink ref="G2" r:id="rId4" xr:uid="{89832B8C-46B1-4E3A-B226-0588FB37741C}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{44E5BE55-9BE8-4C19-8EB2-4729F3ABC777}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{83338F0A-2385-4D32-BE92-53C6E626689D}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
+    <hyperlink ref="G4" r:id="rId8" xr:uid="{CE613E8D-42BF-4A3B-8E64-31449DCA5FFB}"/>
+    <hyperlink ref="E4" r:id="rId9" xr:uid="{90C4CEF0-1AA8-4543-8251-15693CDFF9B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 04-30-2020 21-46-01
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
+++ b/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3914FBDB-80B1-4D6F-B64F-6F69A49DACD2}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B41C5D5D-7C59-4869-862D-3B6F9A4602B2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>Fuente</t>
   </si>
@@ -139,53 +139,69 @@
     <t>16/3/2020</t>
   </si>
   <si>
-    <t>Instituto de seguridad laboral</t>
-  </si>
-  <si>
-    <t>El Instituto de Seguridad Laboral, es la entidad pública encargada de administrar el Seguro Social contra Riesgos de Accidentes del Trabajo y Enfermedades Profesionales. Es un servicio público que pertenece al Ministerio del Trabajo y Previsión Social, y a través de su actuar genera Valor Público otorgando Calidad de Vida a los y las trabajadores/as</t>
-  </si>
-  <si>
-    <t>https://www.isl.gob.cl/covid-19/</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
     <t>secretaría de Gobernación Justicia y Desentralización</t>
   </si>
   <si>
-    <t>Ante la emergencia nacional como prevención ante el COVID-19, se realizó
-la suspensión de labores en dichas Dependencias a partir del lunes dieciséis
-(16) al viernes veinte (20) de marzo del presente año.
-Los días antes mencionados se declaran INHÁBILES para los efectos, plazos,
-actuaciones y términos legales que la Ley establece, los cuales quedan
-suspendidos empezando a correr nuevamente los términos legales a partir
-del primer día hábil.</t>
-  </si>
-  <si>
-    <t>Locales de pago pensionados, sucursales abiertas (Sábado 28 y Domingo 29 Marzo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.ips.gob.cl/servlet/internet/noticia/1421810692952/locales-pago-operativos-sabado28-domingo29-marzo </t>
-  </si>
-  <si>
-    <t>Dirección del trabajo</t>
-  </si>
-  <si>
-    <t>La Dirección del Trabajo es un Servicio Público descentralizado, con personalidad jurídica y patrimonio propio. Está sometido a la supervigilancia del Presidente de la República a través del Ministerio del Trabajo y Previsión Social, y se rige por su Ley Orgánica (D.F.L. Nº 2, del 30 de mayo de 1967) y el D.L. Nº 3.501 de 1981.</t>
-  </si>
-  <si>
-    <t>Centro de consultas COVID-19, preguntas frecuentes.</t>
-  </si>
-  <si>
-    <t>https://www.dt.gob.cl/portal/1628/w3-propertyvalue-178125.html</t>
+    <t>La institución que rectora lo concerniente al gobierno del interior de la república, la gobernabilidad, el acceso a la justicia y  la descentralización, contribuyendo a una  cultura democrática, al desarrollo local,  con transparencia y participación ciudadana, para el bienestar social cultural y el honor de la población en general.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=Comunicados&amp;page=9</t>
+  </si>
+  <si>
+    <t>Ante la emergencia nacional como prevención ante el COVID-19, se realizó la suspensión de labores en dichas Dependencias a partir del lunes dieciséis (16) al viernes veinte (20) de marzo del presente año.
+Los días antes mencionados se declaran INHÁBILES para los efectos, plazos, actuaciones y términos legales que la Ley establece, los cuales quedan suspendidos empezando a correr nuevamente los términos legales a partir del primer día hábil.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=comunicado-secretaria-de-gobernacion-justicia-y-descentralizacion</t>
+  </si>
+  <si>
+    <t>Agencia Hondureña de Aeronáutica Civil.</t>
+  </si>
+  <si>
+    <t>Agencia encargada de vigilancia y supervisión de las operaciones de aviación civil que se desarrollan en la República de Honduras.</t>
+  </si>
+  <si>
+    <t>En marco de la declaracion de emergencia nacional y las ultimas disposiciones emitidas en el Decreto Ejecutivo PCM -021-2020 en el que se decreta la suspensión por siete dias de algunas garantias constitucionales. Se notifica que se dispone el cierre de operaciones de los aeropuertos internacionales.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=comunicado-aeropuertos-de-honduras</t>
+  </si>
+  <si>
+    <t>17/3/2020</t>
+  </si>
+  <si>
+    <t>Administracion Aduanera de Honduras</t>
+  </si>
+  <si>
+    <t>Institución cuya misión es garantizar la facilitación del comercio, la recaudación y la seguridad mediante un control eficiente, utilizando las mejores prácticas a fin de contribuir al aumento y dinamización de la actividad económica del país.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ante el Decreto Ejecutivo PCM 021-2020 se informa lo siguiente: En aras de facilitar el comercio y el ingreso de suministros, los diferentes puntos aduaneros del país estan operando de manera normal en las actividades de comercio exterior de exportacion e importacion de mercancias. </t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=excepcion-para-puntos-aduaneros</t>
+  </si>
+  <si>
+    <t>Secretaría de Desarrollo Económico</t>
+  </si>
+  <si>
+    <t>Secretaria responsable en fomentar el crecimiento en las inversiones y exportaciones en consonancia con la implementación agresiva de la promoción de la imagen y marca país y, de la competitividad, garantizar el acceso en un 100% a los mercados internacionales y la efectividad del funcionamiento del régimen de comercio exterior, facilitar la gestión empresarial, promover la generación de empleo a través del fomento de la competitividad y productividad de las MIPYMES-SSE y velar por la protección de los consumidores</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=congelamiento-de-precios-absoluto</t>
+  </si>
+  <si>
+    <t>18/3/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,14 +249,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="8"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -268,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -304,12 +312,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -329,11 +361,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -355,6 +384,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -786,8 +848,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K7" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K7" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K12" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{A60CF310-D129-4744-AE47-EA0A16C6004B}" name="Fuente" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{CC100997-5BD5-48A6-8DA1-3E422557046E}" name="ID_Dato " dataDxfId="9">
@@ -1104,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1160,7 +1222,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="6">
@@ -1170,19 +1232,19 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1195,7 +1257,7 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6">
@@ -1205,20 +1267,20 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1230,7 +1292,7 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="6">
@@ -1240,19 +1302,19 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="10"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="5" t="s">
         <v>28</v>
       </c>
@@ -1264,7 +1326,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="6">
@@ -1274,28 +1336,32 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="8" t="s">
+      <c r="E5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="10">
-        <v>43917</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="F5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="J5" s="5" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A6" s="11" t="s">
-        <v>33</v>
+      <c r="A6" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="B6" s="6">
         <f t="shared" si="0"/>
@@ -1304,30 +1370,32 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="10">
-        <v>43917</v>
-      </c>
-      <c r="I6" s="5"/>
+      <c r="G6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="J6" s="5" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57.6">
-      <c r="A7" s="11" t="s">
-        <v>37</v>
+    <row r="7" spans="1:12" ht="63.75">
+      <c r="A7" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B7" s="6">
         <f t="shared" si="0"/>
@@ -1336,45 +1404,141 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="10">
-        <v>43917</v>
-      </c>
-      <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="120">
+      <c r="A8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" ref="B8:B12" si="1">+ROW()-1</f>
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75">
+      <c r="A9" s="10"/>
+      <c r="B9" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="18.75">
+      <c r="A10" s="10"/>
+      <c r="B10" s="6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" ht="18.75">
+      <c r="A11" s="10"/>
+      <c r="B11" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="18.75">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C7" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C12" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{0FD97349-53B2-48F9-8FB0-F36688365579}"/>
-    <hyperlink ref="G6" r:id="rId2" display="https://www.ips.gob.cl/servlet/internet/noticia/1421810692952/locales-pago-operativos-sabado28-domingo29-marzo" xr:uid="{153699C3-67F5-46C6-BDEF-5E8F5CECE9F1}"/>
-    <hyperlink ref="G7" r:id="rId3" xr:uid="{A81D850A-A085-4232-A1D2-7280F93E1078}"/>
-    <hyperlink ref="G2" r:id="rId4" xr:uid="{89832B8C-46B1-4E3A-B226-0588FB37741C}"/>
-    <hyperlink ref="E2" r:id="rId5" xr:uid="{44E5BE55-9BE8-4C19-8EB2-4729F3ABC777}"/>
-    <hyperlink ref="G3" r:id="rId6" xr:uid="{83338F0A-2385-4D32-BE92-53C6E626689D}"/>
-    <hyperlink ref="E3" r:id="rId7" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
-    <hyperlink ref="G4" r:id="rId8" xr:uid="{CE613E8D-42BF-4A3B-8E64-31449DCA5FFB}"/>
-    <hyperlink ref="E4" r:id="rId9" xr:uid="{90C4CEF0-1AA8-4543-8251-15693CDFF9B6}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{89832B8C-46B1-4E3A-B226-0588FB37741C}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{44E5BE55-9BE8-4C19-8EB2-4729F3ABC777}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{83338F0A-2385-4D32-BE92-53C6E626689D}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{CE613E8D-42BF-4A3B-8E64-31449DCA5FFB}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{90C4CEF0-1AA8-4543-8251-15693CDFF9B6}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{4E4760D3-6939-4C41-ADE3-E7A46EE0C5BC}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{76EDB031-9D13-49CF-A7FB-527CC4D7B499}"/>
+    <hyperlink ref="G6" r:id="rId9" xr:uid="{C20EEBB6-370E-4FE3-B260-271A29AF1401}"/>
+    <hyperlink ref="E6" r:id="rId10" xr:uid="{DCBF52A4-8079-4083-8EFA-355A40E5133C}"/>
+    <hyperlink ref="G7" r:id="rId11" xr:uid="{27ED4CFC-A676-49E3-8DBF-B96D8241FED5}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{D1755C3C-47A5-4BE1-9969-B7EF3A410A83}"/>
+    <hyperlink ref="G8" r:id="rId13" xr:uid="{90448276-2029-41D4-9F26-EDF75765AFE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 04-30-2020 23-14-45
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
+++ b/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B41C5D5D-7C59-4869-862D-3B6F9A4602B2}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C9496034-E22B-4E87-B3D9-CF8ACFD96A14}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>Fuente</t>
   </si>
@@ -161,7 +161,7 @@
     <t>Agencia encargada de vigilancia y supervisión de las operaciones de aviación civil que se desarrollan en la República de Honduras.</t>
   </si>
   <si>
-    <t>En marco de la declaracion de emergencia nacional y las ultimas disposiciones emitidas en el Decreto Ejecutivo PCM -021-2020 en el que se decreta la suspensión por siete dias de algunas garantias constitucionales. Se notifica que se dispone el cierre de operaciones de los aeropuertos internacionales.</t>
+    <t>En marco de la declaracion de emergencia nacional y las ultimas disposiciones emitidas en el Decreto Ejecutivo PCM -021-2020 en el que se decreta la suspensión  de algunas garantias constitucionales. Se notifica que se dispone el cierre de operaciones de los aeropuertos internacionales.</t>
   </si>
   <si>
     <t>https://covid19honduras.org/?q=comunicado-aeropuertos-de-honduras</t>
@@ -188,10 +188,35 @@
     <t>Secretaria responsable en fomentar el crecimiento en las inversiones y exportaciones en consonancia con la implementación agresiva de la promoción de la imagen y marca país y, de la competitividad, garantizar el acceso en un 100% a los mercados internacionales y la efectividad del funcionamiento del régimen de comercio exterior, facilitar la gestión empresarial, promover la generación de empleo a través del fomento de la competitividad y productividad de las MIPYMES-SSE y velar por la protección de los consumidores</t>
   </si>
   <si>
+    <t>https://covid19honduras.org/?q=Comunicados&amp;page=8</t>
+  </si>
+  <si>
+    <t>El gobierno de la República, a través de la Secretaria de Desarollo Económico, en el marco de la emergencia nacional sanitaria decretada, informa: Para garantizar que no se comentan abusus contra la población, a nivel nacional se decreta congelamiento de preciosos absoluto de los productos de la canasta básica y productos de higiene personal y de hogar.</t>
+  </si>
+  <si>
     <t>https://covid19honduras.org/?q=congelamiento-de-precios-absoluto</t>
   </si>
   <si>
     <t>18/3/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instituto Nacional de Migración </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instituto Nacional de Migración tiene como misión fundamental ejercer el control y regulación como máxima autoridad en materia migratoria a nacionales y extranjeros en el marco de la protección de sus derechos y seguridad, en aplicación de la Ley de Migración y Extranjería y la Política Migratoria del Gobierno de la República, mediante una gestión migratoria moderna, dinámica y transparente.
+ </t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=Comunicados&amp;page=7</t>
+  </si>
+  <si>
+    <t>Siguiendo las disposiciones emitidas por el gobierno de Honduras el INM informa que los puntos de control migratorio se mantienen operando para: 1) Ingreso al país de hondureños residentes y diplomáticos. 2) Salida del terrotoio nacional a extranjeros. 3) Entrada y salida de transportistas de carga unicamente.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=flujos-migratorios</t>
+  </si>
+  <si>
+    <t>21/3/2020</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1439,34 +1464,54 @@
       <c r="D8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="G8" s="25" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="18.75">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:12" ht="120">
+      <c r="A9" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="B9" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="15"/>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="H9" s="16"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:12" ht="18.75">
@@ -1535,10 +1580,13 @@
     <hyperlink ref="G7" r:id="rId11" xr:uid="{27ED4CFC-A676-49E3-8DBF-B96D8241FED5}"/>
     <hyperlink ref="E7" r:id="rId12" xr:uid="{D1755C3C-47A5-4BE1-9969-B7EF3A410A83}"/>
     <hyperlink ref="G8" r:id="rId13" xr:uid="{90448276-2029-41D4-9F26-EDF75765AFE7}"/>
+    <hyperlink ref="E8" r:id="rId14" xr:uid="{61140C4B-261F-49F4-A165-F05ECDA09000}"/>
+    <hyperlink ref="G9" r:id="rId15" xr:uid="{B333F99D-E6A3-441B-91B8-5644745830C4}"/>
+    <hyperlink ref="E9" r:id="rId16" xr:uid="{52316D1F-F875-45D4-BC68-D0EF12900E9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-01-2020 00-42-08
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
+++ b/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C9496034-E22B-4E87-B3D9-CF8ACFD96A14}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2BB0F164-C3E0-423F-A563-3C46DAA70CE7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>Fuente</t>
   </si>
@@ -200,7 +200,7 @@
     <t>18/3/2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Instituto Nacional de Migración </t>
+    <t>Instituto Nacional de Migración (INM)</t>
   </si>
   <si>
     <t xml:space="preserve">Instituto Nacional de Migración tiene como misión fundamental ejercer el control y regulación como máxima autoridad en materia migratoria a nacionales y extranjeros en el marco de la protección de sus derechos y seguridad, en aplicación de la Ley de Migración y Extranjería y la Política Migratoria del Gobierno de la República, mediante una gestión migratoria moderna, dinámica y transparente.
@@ -217,6 +217,30 @@
   </si>
   <si>
     <t>21/3/2020</t>
+  </si>
+  <si>
+    <t>Comision Nacional de Bancos y Seguro (CNBS)</t>
+  </si>
+  <si>
+    <t>Institución que por mandato constitucional tiene la responsabilidad de velar por la estabilidad y solvencia del sistema financiero y demás supervisados, su regulación, supervisión y control. Asimismo, vigilamos la transparencia y que se respeten los derechos de los usuarios financieros, así como coadyuvamos con el sistema de prevención y detección del lavado activos y financiamiento al terrorismo, y contribuimos a promover la educación e inclusión financiera, a fin de salvaguardar el interés público.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=cnbs-22-3</t>
+  </si>
+  <si>
+    <t>Las instituciones por la CNBS que realizan operaciones de crédito, podran otorgar periodos de gracia a los deudores que sean afectados por la reduccion de sus flujos de efectivo los cuales se podran otorgar hasta el 30 de junio de 2020.</t>
+  </si>
+  <si>
+    <t>22/3/2020</t>
+  </si>
+  <si>
+    <t>Secretaria de Trabajo y Seguridad Social</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=secretaria-de-trabajo</t>
+  </si>
+  <si>
+    <t>26/3/2020</t>
   </si>
 </sst>
 </file>
@@ -1193,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1514,36 +1538,64 @@
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="18.75">
-      <c r="A10" s="10"/>
+    <row r="10" spans="1:12" ht="105">
+      <c r="A10" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="B10" s="6">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="18.75">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:12" ht="45">
+      <c r="A11" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="B11" s="6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D11" s="11"/>
       <c r="E11" s="7"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="25" t="s">
+        <v>61</v>
+      </c>
       <c r="H11" s="16"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="18.75">
@@ -1583,10 +1635,13 @@
     <hyperlink ref="E8" r:id="rId14" xr:uid="{61140C4B-261F-49F4-A165-F05ECDA09000}"/>
     <hyperlink ref="G9" r:id="rId15" xr:uid="{B333F99D-E6A3-441B-91B8-5644745830C4}"/>
     <hyperlink ref="E9" r:id="rId16" xr:uid="{52316D1F-F875-45D4-BC68-D0EF12900E9A}"/>
+    <hyperlink ref="G10" r:id="rId17" xr:uid="{F2765C1B-000B-42B0-B842-3A1C402875AF}"/>
+    <hyperlink ref="E10" r:id="rId18" xr:uid="{BF4AAFF6-8642-42F4-B4D4-D27AEF285F0C}"/>
+    <hyperlink ref="G11" r:id="rId19" xr:uid="{90EAA1B8-67AE-4786-9AB7-EFFE2A7274E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-01-2020 02-11-48
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
+++ b/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2BB0F164-C3E0-423F-A563-3C46DAA70CE7}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DEED746F-ECE7-4B8C-9283-06E126783D79}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
   <si>
     <t>Fuente</t>
   </si>
@@ -237,10 +237,64 @@
     <t>Secretaria de Trabajo y Seguridad Social</t>
   </si>
   <si>
+    <t>Secretaría de Trabajo y Seguridad Social de Honduras es el encargado de lo concerniente a la formulación, coordinación, ejecución y evaluación de las políticas de empleo, inclusive de los discapacitados, el salario, la formación de mano de obra, el fomento de la educación obrera y de las relaciones obreras patronales, la inmigración laboral selectiva, la coordinación del sistema de Seguridad Social, el reconocimiento y registro de la personalidad jurídica de Sindicatos y demás organizaciones laborales, lo relativo a la higiene y seguridad ocupacional, el manejo de los procedimientos administrativos de solución de los conflictos individuales y colectivos de trabajo.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=Comunicados&amp;page=6</t>
+  </si>
+  <si>
+    <t>Se autoriza a los empleadores y trabajadores del sector privado para que mediante acuerdo entre las partes convengan que los días feriados señalados en el artículo 339 del Código de Trabajo se consideren como otorgados y gozados por parte de los trabajadores durante el periodo de vigencia del Estado de Emergencia Sanitaria Nacional por la propagación del Covid-19 (Coronavirus).-</t>
+  </si>
+  <si>
     <t>https://covid19honduras.org/?q=secretaria-de-trabajo</t>
   </si>
   <si>
     <t>26/3/2020</t>
+  </si>
+  <si>
+    <t>Economía</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=Comunicados&amp;page=5</t>
+  </si>
+  <si>
+    <t>Establecer el precio máximo en todo el territorio nacional de los productos al consumidor final.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=precios-maximos-canasta-basica</t>
+  </si>
+  <si>
+    <t>27/3/2020</t>
+  </si>
+  <si>
+    <t>BANHPROVI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Economía </t>
+  </si>
+  <si>
+    <t>Institución financiera que contribuye al desarrollo socioeconómico del país y al mejoramiento de la calidad de vida de los hondureños, fomentando y fortaleciendo la inclusión financiera de los beneficiarios.</t>
+  </si>
+  <si>
+    <t>Se realizará la readecuación de todos los préstamos redescontados a las instituciones financieras, mediante el traslado de las cuotas de los meses de marzo, abril y mayo de 2020 creando una ampliación de la fecha de vencimiento del crédito.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=banhprovi</t>
+  </si>
+  <si>
+    <t>24/3/2020</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=Comunicados&amp;page=1</t>
+  </si>
+  <si>
+    <t>Las Empresas que decidan acogerse a las disposiciones de la sección séptima del Decreto Legislativo No. 33-2020, deberán enviar una nota al correo electrónico.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=ley-de-auxilio</t>
+  </si>
+  <si>
+    <t>18/4/2020</t>
   </si>
 </sst>
 </file>
@@ -390,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -466,6 +520,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -897,8 +954,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K12" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K18" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K18" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{A60CF310-D129-4744-AE47-EA0A16C6004B}" name="Fuente" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{CC100997-5BD5-48A6-8DA1-3E422557046E}" name="ID_Dato " dataDxfId="9">
@@ -1215,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1404,9 +1461,7 @@
       <c r="J5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="61.9" customHeight="1">
       <c r="A6" s="10" t="s">
@@ -1572,7 +1627,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="45">
+    <row r="11" spans="1:12" ht="150">
       <c r="A11" s="10" t="s">
         <v>60</v>
       </c>
@@ -1583,40 +1638,192 @@
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="G11" s="25" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:12" ht="120">
+      <c r="A12" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="B12" s="18">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="15"/>
+      <c r="C12" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>69</v>
+      </c>
       <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
+      <c r="I12" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>17</v>
+      </c>
       <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:12" ht="63.75">
+      <c r="A13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="6">
+        <f t="shared" ref="B13:B18" si="2">+ROW()-1</f>
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="150">
+      <c r="A14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="18.75">
+      <c r="A15" s="10"/>
+      <c r="B15" s="6">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="18.75">
+      <c r="A16" s="10"/>
+      <c r="B16" s="6">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="18.75">
+      <c r="A17" s="10"/>
+      <c r="B17" s="6">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" ht="18.75">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C12" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C18" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{89832B8C-46B1-4E3A-B226-0588FB37741C}"/>
@@ -1638,10 +1845,17 @@
     <hyperlink ref="G10" r:id="rId17" xr:uid="{F2765C1B-000B-42B0-B842-3A1C402875AF}"/>
     <hyperlink ref="E10" r:id="rId18" xr:uid="{BF4AAFF6-8642-42F4-B4D4-D27AEF285F0C}"/>
     <hyperlink ref="G11" r:id="rId19" xr:uid="{90EAA1B8-67AE-4786-9AB7-EFFE2A7274E9}"/>
+    <hyperlink ref="E11" r:id="rId20" xr:uid="{16313C5E-575A-4E7B-9020-293E4E52A652}"/>
+    <hyperlink ref="G12" r:id="rId21" xr:uid="{7245FDFD-2CBD-47B4-93DF-91FF93243F7E}"/>
+    <hyperlink ref="E12" r:id="rId22" xr:uid="{D11C0F98-DCAB-4BBA-A8DC-4E2B66805B18}"/>
+    <hyperlink ref="G13" r:id="rId23" xr:uid="{8C650575-6C55-44BD-A0BA-59EFE971353F}"/>
+    <hyperlink ref="E13" r:id="rId24" xr:uid="{B0E6EF00-013B-46E0-A9D8-D76A7488E3F0}"/>
+    <hyperlink ref="G14" r:id="rId25" xr:uid="{D888ED92-439A-42B0-91EF-7BD2E8F09DE8}"/>
+    <hyperlink ref="E14" r:id="rId26" xr:uid="{249E9D6C-C4E9-48FF-89C0-9FE1AC968A21}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-01-2020 03-29-19
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
+++ b/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DEED746F-ECE7-4B8C-9283-06E126783D79}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AC9E7C0B-30C1-4A7E-AB25-EBC2370F9862}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -304,7 +304,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,13 +346,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -444,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -464,9 +457,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -488,9 +478,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -504,9 +491,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -954,8 +938,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K18" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K18" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K14" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{A60CF310-D129-4744-AE47-EA0A16C6004B}" name="Fuente" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{CC100997-5BD5-48A6-8DA1-3E422557046E}" name="ID_Dato " dataDxfId="9">
@@ -1274,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1328,7 +1312,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="6">
@@ -1338,19 +1322,19 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1363,7 +1347,7 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6">
@@ -1373,20 +1357,20 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1398,7 +1382,7 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="6">
@@ -1408,19 +1392,19 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
         <v>28</v>
       </c>
@@ -1432,7 +1416,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="6">
@@ -1442,19 +1426,19 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="5" t="s">
         <v>28</v>
       </c>
@@ -1464,7 +1448,7 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="61.9" customHeight="1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="6">
@@ -1474,19 +1458,19 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="5" t="s">
         <v>38</v>
       </c>
@@ -1498,7 +1482,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="63.75">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="6">
@@ -1508,19 +1492,19 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="5" t="s">
         <v>38</v>
       </c>
@@ -1530,7 +1514,7 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:12" ht="120">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="6">
@@ -1540,19 +1524,19 @@
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="5" t="s">
         <v>48</v>
       </c>
@@ -1562,7 +1546,7 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:12" ht="120">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="6">
@@ -1572,19 +1556,19 @@
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="16"/>
+      <c r="H9" s="14"/>
       <c r="I9" s="5" t="s">
         <v>54</v>
       </c>
@@ -1594,7 +1578,7 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:12" ht="105">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="6">
@@ -1604,19 +1588,19 @@
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="14" t="s">
         <v>54</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -1628,7 +1612,7 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:12" ht="150">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="6">
@@ -1638,19 +1622,19 @@
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="5" t="s">
         <v>65</v>
       </c>
@@ -1660,61 +1644,61 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="120">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="16">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="20"/>
+      <c r="I12" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="24"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:12" ht="63.75">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="6">
-        <f t="shared" ref="B13:B18" si="2">+ROW()-1</f>
+        <f t="shared" ref="B13:B14" si="2">+ROW()-1</f>
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="14" t="s">
         <v>76</v>
       </c>
       <c r="I13" s="5" t="s">
@@ -1726,7 +1710,7 @@
       <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="150">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="6">
@@ -1736,19 +1720,19 @@
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="16"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="5" t="s">
         <v>80</v>
       </c>
@@ -1757,73 +1741,13 @@
       </c>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="18.75">
-      <c r="A15" s="10"/>
-      <c r="B15" s="6">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" ht="18.75">
-      <c r="A16" s="10"/>
-      <c r="B16" s="6">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" ht="18.75">
-      <c r="A17" s="10"/>
-      <c r="B17" s="6">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" ht="18.75">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-    </row>
+    <row r="15" spans="1:12" ht="15"/>
+    <row r="16" spans="1:12" ht="15"/>
+    <row r="17" ht="15"/>
+    <row r="18" ht="15"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C18" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C14" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{89832B8C-46B1-4E3A-B226-0588FB37741C}"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-05-2020 01-58-00
</commit_message>
<xml_diff>
--- a/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
+++ b/datacovidhn/00 DATACOVID Trabajo_HN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22823"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000 DRIVE\000 DATACOVID HN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AC9E7C0B-30C1-4A7E-AB25-EBC2370F9862}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2754B88-E2F4-4212-81A8-AF673305AE9C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>16/3/2020</t>
   </si>
   <si>
-    <t>secretaría de Gobernación Justicia y Desentralización</t>
-  </si>
-  <si>
     <t>La institución que rectora lo concerniente al gobierno del interior de la república, la gobernabilidad, el acceso a la justicia y  la descentralización, contribuyendo a una  cultura democrática, al desarrollo local,  con transparencia y participación ciudadana, para el bienestar social cultural y el honor de la población en general.</t>
   </si>
   <si>
@@ -295,16 +292,16 @@
   </si>
   <si>
     <t>18/4/2020</t>
+  </si>
+  <si>
+    <t>Secretaría de Gobernación Justicia y Desentralización</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-  </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -478,7 +475,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -496,7 +493,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -508,9 +505,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -520,7 +520,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -564,7 +564,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="4"/>
@@ -581,7 +581,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -811,13 +811,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4"/>
         </left>
@@ -839,6 +832,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -938,7 +938,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A1:K14" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{A60CF310-D129-4744-AE47-EA0A16C6004B}" name="Fuente" dataDxfId="10"/>
@@ -952,15 +952,15 @@
     <tableColumn id="10" xr3:uid="{C428BE36-6D12-4F4C-937B-4D9B2BE733CB}" name="Sitio Web" dataDxfId="4"/>
     <tableColumn id="14" xr3:uid="{8A64974B-7039-4EC2-86FD-F906B25B65C5}" name="Fecha consulta" dataDxfId="3"/>
     <tableColumn id="15" xr3:uid="{76A5A7F7-E8CD-4AD7-BD38-521CEC7FA43D}" name="Fecha publicación" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{C1BACFD5-672A-458F-A24A-AF2164F6B966}" name="País" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{CBA3644C-97A1-4B18-A3FF-89F9754FAC27}" name="División administrativa" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{C1BACFD5-672A-458F-A24A-AF2164F6B966}" name="País" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{CBA3644C-97A1-4B18-A3FF-89F9754FAC27}" name="División administrativa" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1256,27 +1256,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="69.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="55.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="69.109375" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="6" max="6" width="55.33203125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="11" max="11" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.9" thickBot="1">
+    <row r="1" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="61.9" customHeight="1">
+    <row r="2" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="61.9" customHeight="1">
+    <row r="3" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="61.9" customHeight="1">
+    <row r="4" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
@@ -1405,19 +1405,19 @@
         <v>27</v>
       </c>
       <c r="H4" s="8"/>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="61.9" customHeight="1">
+    <row r="5" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="B5" s="6">
         <f t="shared" si="0"/>
@@ -1427,29 +1427,29 @@
         <v>12</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="H5" s="8"/>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="61.9" customHeight="1">
+    <row r="6" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6">
         <f t="shared" si="0"/>
@@ -1459,31 +1459,31 @@
         <v>12</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="63.75">
+    <row r="7" spans="1:12" ht="69" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="6">
         <f t="shared" si="0"/>
@@ -1493,29 +1493,29 @@
         <v>12</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="H7" s="8"/>
-      <c r="I7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="I7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="120">
+    <row r="8" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6">
         <f t="shared" ref="B8:B12" si="1">+ROW()-1</f>
@@ -1525,29 +1525,29 @@
         <v>12</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="H8" s="14"/>
+      <c r="I8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="120">
+    <row r="9" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="6">
         <f t="shared" si="1"/>
@@ -1557,29 +1557,29 @@
         <v>12</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="105">
+    <row r="10" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="6">
         <f t="shared" si="1"/>
@@ -1589,31 +1589,31 @@
         <v>12</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="150">
+    <row r="11" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="6">
         <f t="shared" si="1"/>
@@ -1623,95 +1623,95 @@
         <v>12</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="H11" s="14"/>
+      <c r="I11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="120">
+    <row r="12" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="16">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C12" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="23" t="s">
+      <c r="F12" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="G12" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="H12" s="20"/>
+      <c r="I12" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="24" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="63.75">
+    <row r="13" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="6">
         <f t="shared" ref="B13:B14" si="2">+ROW()-1</f>
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="H13" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="I13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="150">
+    <row r="14" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="6">
         <f t="shared" si="2"/>
@@ -1721,30 +1721,26 @@
         <v>12</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="G14" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="H14" s="14"/>
+      <c r="I14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="15"/>
-    <row r="16" spans="1:12" ht="15"/>
-    <row r="17" ht="15"/>
-    <row r="18" ht="15"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C14" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>

</xml_diff>